<commit_message>
restructuracion de app para cambiar a apis
</commit_message>
<xml_diff>
--- a/public/formatos/remuneracion_import.xlsx
+++ b/public/formatos/remuneracion_import.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Worksheet" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Worksheet!$A$1:$Y$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Worksheet!$A$1:$Z$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">numero_de_documento</t>
   </si>
@@ -32,14 +32,22 @@
   </si>
   <si>
     <t xml:space="preserve">categoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="@_"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -120,12 +128,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -150,99 +166,104 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I:I"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="19.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="4" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1021" style="0" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="4" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1021" min="11" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1022" style="0" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="1" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="n">
+      <c r="E1" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="n">
+      <c r="G1" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="n">
+      <c r="H1" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="n">
+      <c r="I1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="n">
+      <c r="L1" s="2" t="n">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="n">
+      <c r="M1" s="2" t="n">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="n">
+      <c r="N1" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="n">
+      <c r="O1" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="n">
+      <c r="P1" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="n">
+      <c r="Q1" s="2" t="n">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="n">
+      <c r="R1" s="2" t="n">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="n">
+      <c r="S1" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="n">
+      <c r="T1" s="2" t="n">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="n">
+      <c r="U1" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="n">
+      <c r="V1" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="V1" s="1" t="n">
+      <c r="W1" s="2" t="n">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="n">
+      <c r="X1" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="X1" s="1" t="n">
+      <c r="Y1" s="2" t="n">
         <v>21</v>
       </c>
-      <c r="Y1" s="1" t="n">
+      <c r="Z1" s="2" t="n">
         <v>22</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Y1"/>
+  <autoFilter ref="A1:Z1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>